<commit_message>
AIP-980 AIP-1093 Test Data File
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/CAM_763.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/CAM_763.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD336F3-9E29-4420-8480-AC5C85F530E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4AD2C6-E31F-436B-8533-81295AFBA979}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20616" yWindow="-120" windowWidth="20736" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>DeviceName</t>
   </si>
@@ -100,7 +100,13 @@
     <t>800</t>
   </si>
   <si>
-    <t>ExpectedRecordDuration_1</t>
+    <t>OmicronFile</t>
+  </si>
+  <si>
+    <t>CAM_763.seq</t>
+  </si>
+  <si>
+    <t>ExpectedRecordDuration</t>
   </si>
 </sst>
 </file>
@@ -422,41 +428,41 @@
   <dimension ref="A1:AI3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="16.88671875" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="16.85546875" customWidth="1"/>
     <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="14" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="28" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -503,10 +509,13 @@
         <v>18</v>
       </c>
       <c r="P1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -555,7 +564,9 @@
       <c r="P2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" s="1"/>
+      <c r="Q2" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -570,7 +581,7 @@
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="F3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>

</xml_diff>